<commit_message>
Update Data Transformation Process and Plan.xlsx
</commit_message>
<xml_diff>
--- a/Resources/Raw Data/Data Transformation Process and Plan.xlsx
+++ b/Resources/Raw Data/Data Transformation Process and Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navyh\OneDrive\Desktop\U of T BootCamp\Homework\Unit 6 - Project 1\CanadaEnergyIE\Resources\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D32C8C-6B2C-43BE-825A-BA1A1D20A8D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D003164C-B4A9-48F0-8635-A8B934F5F460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9B33D0E1-F168-4917-B233-3C6CBB1CDC02}"/>
   </bookViews>
@@ -754,14 +754,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -771,9 +777,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -789,9 +792,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -31978,72 +31978,72 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="36"/>
-      <c r="P2" s="30" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="37"/>
+      <c r="P2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="32"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="34"/>
     </row>
     <row r="3" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="P3" s="33" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="P3" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="33"/>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="33"/>
-      <c r="AA3" s="33"/>
-      <c r="AB3" s="33"/>
-      <c r="AC3" s="33"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="27"/>
     </row>
     <row r="4" spans="1:29" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -32091,43 +32091,43 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
       <c r="Q8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
       <c r="P9">
         <v>2</v>
       </c>
@@ -32151,22 +32151,22 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="30" t="s">
+      <c r="P10" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="31"/>
-      <c r="X10" s="31"/>
-      <c r="Y10" s="31"/>
-      <c r="Z10" s="31"/>
-      <c r="AA10" s="31"/>
-      <c r="AB10" s="31"/>
-      <c r="AC10" s="32"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="34"/>
     </row>
     <row r="11" spans="1:29" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
@@ -32211,22 +32211,22 @@
       <c r="N11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="33" t="s">
+      <c r="P11" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="33"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="33"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="33"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="27"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
@@ -32393,22 +32393,22 @@
       </c>
     </row>
     <row r="18" spans="1:29" ht="21" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
       <c r="P18">
         <v>1</v>
       </c>
@@ -32417,22 +32417,22 @@
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
       <c r="P19">
         <v>2</v>
       </c>
@@ -32503,74 +32503,74 @@
       <c r="AC22" s="1"/>
     </row>
     <row r="23" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="38" t="s">
+      <c r="P23" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="38"/>
-      <c r="X23" s="38"/>
-      <c r="Y23" s="38"/>
-      <c r="Z23" s="38"/>
-      <c r="AA23" s="38"/>
-      <c r="AB23" s="38"/>
-      <c r="AC23" s="38"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="39"/>
+      <c r="X23" s="39"/>
+      <c r="Y23" s="39"/>
+      <c r="Z23" s="39"/>
+      <c r="AA23" s="39"/>
+      <c r="AB23" s="39"/>
+      <c r="AC23" s="39"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="33" t="s">
+      <c r="P24" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="33"/>
-      <c r="W24" s="33"/>
-      <c r="X24" s="33"/>
-      <c r="Y24" s="33"/>
-      <c r="Z24" s="33"/>
-      <c r="AA24" s="33"/>
-      <c r="AB24" s="33"/>
-      <c r="AC24" s="33"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
+      <c r="AA24" s="27"/>
+      <c r="AB24" s="27"/>
+      <c r="AC24" s="27"/>
     </row>
     <row r="25" spans="1:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -32584,21 +32584,21 @@
       <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
       <c r="P26" s="17" t="s">
         <v>77</v>
       </c>
@@ -32895,74 +32895,74 @@
       <c r="AC38" s="1"/>
     </row>
     <row r="39" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="29"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
       <c r="O39" s="10"/>
-      <c r="P39" s="29" t="s">
+      <c r="P39" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="Q39" s="29"/>
-      <c r="R39" s="29"/>
-      <c r="S39" s="29"/>
-      <c r="T39" s="29"/>
-      <c r="U39" s="29"/>
-      <c r="V39" s="29"/>
-      <c r="W39" s="29"/>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="29"/>
-      <c r="AC39" s="29"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="28"/>
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
+      <c r="Z39" s="28"/>
+      <c r="AA39" s="28"/>
+      <c r="AB39" s="28"/>
+      <c r="AC39" s="28"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
       <c r="O40" s="11"/>
-      <c r="P40" s="33" t="s">
+      <c r="P40" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="Q40" s="33"/>
-      <c r="R40" s="33"/>
-      <c r="S40" s="33"/>
-      <c r="T40" s="33"/>
-      <c r="U40" s="33"/>
-      <c r="V40" s="33"/>
-      <c r="W40" s="33"/>
-      <c r="X40" s="33"/>
-      <c r="Y40" s="33"/>
-      <c r="Z40" s="33"/>
-      <c r="AA40" s="33"/>
-      <c r="AB40" s="33"/>
-      <c r="AC40" s="33"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27"/>
+      <c r="U40" s="27"/>
+      <c r="V40" s="27"/>
+      <c r="W40" s="27"/>
+      <c r="X40" s="27"/>
+      <c r="Y40" s="27"/>
+      <c r="Z40" s="27"/>
+      <c r="AA40" s="27"/>
+      <c r="AB40" s="27"/>
+      <c r="AC40" s="27"/>
     </row>
     <row r="41" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
@@ -33129,15 +33129,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A40:N40"/>
-    <mergeCell ref="P39:AC39"/>
-    <mergeCell ref="P40:AC40"/>
-    <mergeCell ref="A18:N18"/>
-    <mergeCell ref="A19:N19"/>
-    <mergeCell ref="A24:N24"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="P24:AC24"/>
-    <mergeCell ref="A39:N39"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A9:N9"/>
     <mergeCell ref="A23:N23"/>
@@ -33148,6 +33139,15 @@
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="P23:AC23"/>
+    <mergeCell ref="A40:N40"/>
+    <mergeCell ref="P39:AC39"/>
+    <mergeCell ref="P40:AC40"/>
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A24:N24"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="P24:AC24"/>
+    <mergeCell ref="A39:N39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q32" r:id="rId1" xr:uid="{DB482FDF-A08F-441B-B744-36C17301768B}"/>
@@ -33235,8 +33235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351174CB-81E9-4D52-A08A-5E76FD1732BF}">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y40" sqref="Y40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Table 1 in csv format
</commit_message>
<xml_diff>
--- a/Resources/Raw Data/Data Transformation Process and Plan.xlsx
+++ b/Resources/Raw Data/Data Transformation Process and Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navyh\OneDrive\Desktop\U of T BootCamp\Homework\Unit 6 - Project 1\CanadaEnergyIE\Resources\Raw Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e23db62feec2a5d/Desktop/U of T BootCamp/Homework/Unit 6 - Project 1/CanadaEnergyIE/Resources/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D003164C-B4A9-48F0-8635-A8B934F5F460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{D003164C-B4A9-48F0-8635-A8B934F5F460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE6B7DCA-116D-4D5D-A762-CC16AA7F79A6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9B33D0E1-F168-4917-B233-3C6CBB1CDC02}"/>
+    <workbookView xWindow="9960" yWindow="876" windowWidth="13848" windowHeight="11460" activeTab="2" xr2:uid="{9B33D0E1-F168-4917-B233-3C6CBB1CDC02}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="153">
   <si>
     <t>Resources</t>
   </si>
@@ -496,6 +496,54 @@
   <si>
     <t>API</t>
   </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>- Set start date, end date, loop through each row, pull just the dates wanted</t>
+  </si>
+  <si>
+    <t>- Table 3:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Table 1: </t>
+  </si>
+  <si>
+    <t>- Delete 1st 2 rows</t>
+  </si>
+  <si>
+    <t>- Delete 1st 15 rows</t>
+  </si>
+  <si>
+    <t>- Merge table 1 with Table 3, on Date</t>
+  </si>
+  <si>
+    <t>- Table 7:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Remove 1st 4 rows </t>
+  </si>
+  <si>
+    <t>- Transpose</t>
+  </si>
+  <si>
+    <t>- New column, combine Quarter with years</t>
+  </si>
+  <si>
+    <t>- Pull Oil column</t>
+  </si>
+  <si>
+    <t>- Merge with Table 3 based on Quarter basis</t>
+  </si>
+  <si>
+    <t>-Plots:</t>
+  </si>
+  <si>
+    <t>- Oil Export vs. USD on Monthly Basis</t>
+  </si>
+  <si>
+    <t>- Oil Export GDP vs. USD onQuarterly basi</t>
+  </si>
 </sst>
 </file>
 
@@ -701,7 +749,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -754,20 +802,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -777,6 +819,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -793,9 +838,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -31978,72 +32027,72 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="37"/>
-      <c r="P2" s="32" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="36"/>
+      <c r="P2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="34"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="32"/>
     </row>
     <row r="3" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="P3" s="27" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="P3" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
-      <c r="AC3" s="27"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="33"/>
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="33"/>
     </row>
     <row r="4" spans="1:29" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -32091,43 +32140,43 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
       <c r="Q8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
       <c r="P9">
         <v>2</v>
       </c>
@@ -32151,22 +32200,22 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="32" t="s">
+      <c r="P10" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="33"/>
-      <c r="T10" s="33"/>
-      <c r="U10" s="33"/>
-      <c r="V10" s="33"/>
-      <c r="W10" s="33"/>
-      <c r="X10" s="33"/>
-      <c r="Y10" s="33"/>
-      <c r="Z10" s="33"/>
-      <c r="AA10" s="33"/>
-      <c r="AB10" s="33"/>
-      <c r="AC10" s="34"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
+      <c r="AC10" s="32"/>
     </row>
     <row r="11" spans="1:29" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
@@ -32211,22 +32260,22 @@
       <c r="N11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="27" t="s">
+      <c r="P11" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="27"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="33"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="33"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
@@ -32393,22 +32442,22 @@
       </c>
     </row>
     <row r="18" spans="1:29" ht="21" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
       <c r="P18">
         <v>1</v>
       </c>
@@ -32417,22 +32466,22 @@
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
       <c r="P19">
         <v>2</v>
       </c>
@@ -32503,74 +32552,74 @@
       <c r="AC22" s="1"/>
     </row>
     <row r="23" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="39" t="s">
+      <c r="P23" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
-      <c r="U23" s="39"/>
-      <c r="V23" s="39"/>
-      <c r="W23" s="39"/>
-      <c r="X23" s="39"/>
-      <c r="Y23" s="39"/>
-      <c r="Z23" s="39"/>
-      <c r="AA23" s="39"/>
-      <c r="AB23" s="39"/>
-      <c r="AC23" s="39"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="38"/>
+      <c r="U23" s="38"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="38"/>
+      <c r="Y23" s="38"/>
+      <c r="Z23" s="38"/>
+      <c r="AA23" s="38"/>
+      <c r="AB23" s="38"/>
+      <c r="AC23" s="38"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="27" t="s">
+      <c r="P24" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="27"/>
-      <c r="AA24" s="27"/>
-      <c r="AB24" s="27"/>
-      <c r="AC24" s="27"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="33"/>
+      <c r="Y24" s="33"/>
+      <c r="Z24" s="33"/>
+      <c r="AA24" s="33"/>
+      <c r="AB24" s="33"/>
+      <c r="AC24" s="33"/>
     </row>
     <row r="25" spans="1:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -32584,21 +32633,21 @@
       <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
       <c r="P26" s="17" t="s">
         <v>77</v>
       </c>
@@ -32895,74 +32944,74 @@
       <c r="AC38" s="1"/>
     </row>
     <row r="39" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
       <c r="O39" s="10"/>
-      <c r="P39" s="28" t="s">
+      <c r="P39" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="Q39" s="28"/>
-      <c r="R39" s="28"/>
-      <c r="S39" s="28"/>
-      <c r="T39" s="28"/>
-      <c r="U39" s="28"/>
-      <c r="V39" s="28"/>
-      <c r="W39" s="28"/>
-      <c r="X39" s="28"/>
-      <c r="Y39" s="28"/>
-      <c r="Z39" s="28"/>
-      <c r="AA39" s="28"/>
-      <c r="AB39" s="28"/>
-      <c r="AC39" s="28"/>
+      <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29"/>
+      <c r="T39" s="29"/>
+      <c r="U39" s="29"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="29"/>
+      <c r="AC39" s="29"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
       <c r="O40" s="11"/>
-      <c r="P40" s="27" t="s">
+      <c r="P40" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="Q40" s="27"/>
-      <c r="R40" s="27"/>
-      <c r="S40" s="27"/>
-      <c r="T40" s="27"/>
-      <c r="U40" s="27"/>
-      <c r="V40" s="27"/>
-      <c r="W40" s="27"/>
-      <c r="X40" s="27"/>
-      <c r="Y40" s="27"/>
-      <c r="Z40" s="27"/>
-      <c r="AA40" s="27"/>
-      <c r="AB40" s="27"/>
-      <c r="AC40" s="27"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="33"/>
+      <c r="S40" s="33"/>
+      <c r="T40" s="33"/>
+      <c r="U40" s="33"/>
+      <c r="V40" s="33"/>
+      <c r="W40" s="33"/>
+      <c r="X40" s="33"/>
+      <c r="Y40" s="33"/>
+      <c r="Z40" s="33"/>
+      <c r="AA40" s="33"/>
+      <c r="AB40" s="33"/>
+      <c r="AC40" s="33"/>
     </row>
     <row r="41" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
@@ -33129,6 +33178,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A40:N40"/>
+    <mergeCell ref="P39:AC39"/>
+    <mergeCell ref="P40:AC40"/>
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A24:N24"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="P24:AC24"/>
+    <mergeCell ref="A39:N39"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A9:N9"/>
     <mergeCell ref="A23:N23"/>
@@ -33139,15 +33197,6 @@
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="P23:AC23"/>
-    <mergeCell ref="A40:N40"/>
-    <mergeCell ref="P39:AC39"/>
-    <mergeCell ref="P40:AC40"/>
-    <mergeCell ref="A18:N18"/>
-    <mergeCell ref="A19:N19"/>
-    <mergeCell ref="A24:N24"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="P24:AC24"/>
-    <mergeCell ref="A39:N39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q32" r:id="rId1" xr:uid="{DB482FDF-A08F-441B-B744-36C17301768B}"/>
@@ -33233,15 +33282,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351174CB-81E9-4D52-A08A-5E76FD1732BF}">
-  <dimension ref="A1:W59"/>
+  <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y40" sqref="Y40"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>114</v>
       </c>
@@ -33269,45 +33318,103 @@
       <c r="U1" s="7"/>
       <c r="V1" s="7"/>
       <c r="W1" s="7"/>
+      <c r="Y1" t="s">
+        <v>137</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y2" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z2" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Q3" s="24" t="s">
         <v>127</v>
       </c>
+      <c r="Z3" s="41" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y4" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z4" s="41" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z5" s="41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R6" s="40" t="s">
         <v>129</v>
       </c>
       <c r="S6" s="40"/>
       <c r="T6" s="40"/>
+      <c r="Y6" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z6" s="41" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R7" s="40"/>
       <c r="S7" s="40"/>
       <c r="T7" s="40"/>
+      <c r="Z7" s="41" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R8" s="40"/>
       <c r="S8" s="40"/>
       <c r="T8" s="40"/>
+      <c r="Z8" s="41" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R9" s="40"/>
       <c r="S9" s="40"/>
       <c r="T9" s="40"/>
+      <c r="Z9" s="41" t="s">
+        <v>148</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R10" s="40"/>
       <c r="S10" s="40"/>
       <c r="T10" s="40"/>
+      <c r="Z10" s="41" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y11" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z11" s="41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z12" s="41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="K14" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Revert "Update Data Transformation Process and Plan.xlsx"
This reverts commit 1318385c9c9e3e083cc5c2b00aed5d12aa3583d4.
</commit_message>
<xml_diff>
--- a/Resources/Raw Data/Data Transformation Process and Plan.xlsx
+++ b/Resources/Raw Data/Data Transformation Process and Plan.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{D003164C-B4A9-48F0-8635-A8B934F5F460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE6B7DCA-116D-4D5D-A762-CC16AA7F79A6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9B33D0E1-F168-4917-B233-3C6CBB1CDC02}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13848" windowHeight="11460" activeTab="2" xr2:uid="{9B33D0E1-F168-4917-B233-3C6CBB1CDC02}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -803,14 +803,20 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -820,9 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,9 +841,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -32027,72 +32027,72 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="37"/>
-      <c r="P2" s="31" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="38"/>
+      <c r="P2" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="33"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="35"/>
     </row>
     <row r="3" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="P3" s="34" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="P3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="34"/>
-      <c r="Z3" s="34"/>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="34"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
     </row>
     <row r="4" spans="1:29" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -32140,43 +32140,43 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
       <c r="Q8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
       <c r="P9">
         <v>2</v>
       </c>
@@ -32200,22 +32200,22 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="31" t="s">
+      <c r="P10" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="32"/>
-      <c r="AC10" s="33"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="34"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="34"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="35"/>
     </row>
     <row r="11" spans="1:29" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
@@ -32260,22 +32260,22 @@
       <c r="N11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="34" t="s">
+      <c r="P11" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34"/>
-      <c r="U11" s="34"/>
-      <c r="V11" s="34"/>
-      <c r="W11" s="34"/>
-      <c r="X11" s="34"/>
-      <c r="Y11" s="34"/>
-      <c r="Z11" s="34"/>
-      <c r="AA11" s="34"/>
-      <c r="AB11" s="34"/>
-      <c r="AC11" s="34"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="28"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
@@ -32442,22 +32442,22 @@
       </c>
     </row>
     <row r="18" spans="1:29" ht="21" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
       <c r="P18">
         <v>1</v>
       </c>
@@ -32466,22 +32466,22 @@
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
       <c r="P19">
         <v>2</v>
       </c>
@@ -32552,74 +32552,74 @@
       <c r="AC22" s="1"/>
     </row>
     <row r="23" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="39" t="s">
+      <c r="P23" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
-      <c r="U23" s="39"/>
-      <c r="V23" s="39"/>
-      <c r="W23" s="39"/>
-      <c r="X23" s="39"/>
-      <c r="Y23" s="39"/>
-      <c r="Z23" s="39"/>
-      <c r="AA23" s="39"/>
-      <c r="AB23" s="39"/>
-      <c r="AC23" s="39"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="40"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="40"/>
+      <c r="Z23" s="40"/>
+      <c r="AA23" s="40"/>
+      <c r="AB23" s="40"/>
+      <c r="AC23" s="40"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="34" t="s">
+      <c r="P24" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="34"/>
-      <c r="V24" s="34"/>
-      <c r="W24" s="34"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="34"/>
-      <c r="Z24" s="34"/>
-      <c r="AA24" s="34"/>
-      <c r="AB24" s="34"/>
-      <c r="AC24" s="34"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="28"/>
+      <c r="Z24" s="28"/>
+      <c r="AA24" s="28"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="28"/>
     </row>
     <row r="25" spans="1:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -32633,21 +32633,21 @@
       <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="40"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
       <c r="P26" s="17" t="s">
         <v>77</v>
       </c>
@@ -32944,74 +32944,74 @@
       <c r="AC38" s="1"/>
     </row>
     <row r="39" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
       <c r="O39" s="10"/>
-      <c r="P39" s="30" t="s">
+      <c r="P39" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
-      <c r="S39" s="30"/>
-      <c r="T39" s="30"/>
-      <c r="U39" s="30"/>
-      <c r="V39" s="30"/>
-      <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="30"/>
-      <c r="AC39" s="30"/>
+      <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29"/>
+      <c r="T39" s="29"/>
+      <c r="U39" s="29"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="29"/>
+      <c r="AC39" s="29"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
       <c r="O40" s="11"/>
-      <c r="P40" s="34" t="s">
+      <c r="P40" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="34"/>
-      <c r="S40" s="34"/>
-      <c r="T40" s="34"/>
-      <c r="U40" s="34"/>
-      <c r="V40" s="34"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="34"/>
-      <c r="AA40" s="34"/>
-      <c r="AB40" s="34"/>
-      <c r="AC40" s="34"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="28"/>
+      <c r="W40" s="28"/>
+      <c r="X40" s="28"/>
+      <c r="Y40" s="28"/>
+      <c r="Z40" s="28"/>
+      <c r="AA40" s="28"/>
+      <c r="AB40" s="28"/>
+      <c r="AC40" s="28"/>
     </row>
     <row r="41" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
@@ -33178,15 +33178,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A40:N40"/>
-    <mergeCell ref="P39:AC39"/>
-    <mergeCell ref="P40:AC40"/>
-    <mergeCell ref="A18:N18"/>
-    <mergeCell ref="A19:N19"/>
-    <mergeCell ref="A24:N24"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="P24:AC24"/>
-    <mergeCell ref="A39:N39"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A9:N9"/>
     <mergeCell ref="A23:N23"/>
@@ -33197,6 +33188,15 @@
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="P23:AC23"/>
+    <mergeCell ref="A40:N40"/>
+    <mergeCell ref="P39:AC39"/>
+    <mergeCell ref="P40:AC40"/>
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A24:N24"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="P24:AC24"/>
+    <mergeCell ref="A39:N39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q32" r:id="rId1" xr:uid="{DB482FDF-A08F-441B-B744-36C17301768B}"/>

</xml_diff>